<commit_message>
Adding inquiring questions to the SIQ document as it required for not having ambigity about the system design Final review with minor changes (v1.2.1) Signed-off-by: MS2017A <aeronautics2017@gmail.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/Input documents/PO4_DGELV_DIGITAL ELEVATOR_SIQ.xlsx
+++ b/Digital_Elevator_PO4_DGELV/Input documents/PO4_DGELV_DIGITAL ELEVATOR_SIQ.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\Input documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SWE\clone\Digital_Elevator_PO4_DGELV\Input documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66552187-D812-4F52-8B19-65D9B7948630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC5AC2B-1892-46E5-8478-7870CCF67EA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Initiation Phase</t>
   </si>
@@ -56,6 +56,158 @@
   <si>
     <t>Reference Questions (SIQ ID)</t>
   </si>
+  <si>
+    <t>Using lock system at each level or just one system only at the ground level?</t>
+  </si>
+  <si>
+    <t>REQ_ PO4_DGELV _CYRS_07_V1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Reset system inside the elvator room or outside?</t>
+  </si>
+  <si>
+    <t>REQ_ PO4_DGELV _CYRS_06_V1.2</t>
+  </si>
+  <si>
+    <t>What's the number of the level the elevator should work with?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The system has locking subsystem for logging using username and password for 10 users. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>#imp SW</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When the user login correctly and select the level to move to, the Motor should be turned on with the specified direction. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>#imp SW</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">System is switched between On and Off state upon pressing the On/Off push button while a reset for the whole system is done upon holding the On/Off button for 2 sec. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>#imp SW</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SIQ_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PO4_DGELV _01_V1.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SIQ_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PO4_DGELV _02_V1.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SIQ_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PO4_DGELV _03_V1.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>REQ_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PO4_DGELV _CYRS_01_V1.2</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -64,7 +216,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -96,6 +248,43 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -164,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -190,6 +379,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -411,20 +612,20 @@
     <tabColor rgb="FFF2F2F2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD996"/>
+  <dimension ref="A1:AD997"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.36328125" customWidth="1"/>
-    <col min="2" max="2" width="26.6328125" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.7265625" customWidth="1"/>
     <col min="4" max="4" width="21.90625" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="5" max="5" width="34.6328125" customWidth="1"/>
     <col min="6" max="6" width="17.26953125" customWidth="1"/>
     <col min="7" max="7" width="16.54296875" customWidth="1"/>
     <col min="8" max="8" width="10.36328125" customWidth="1"/>
@@ -519,12 +720,20 @@
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
     </row>
-    <row r="3" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="45.6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="11"/>
+      <c r="B3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F3" s="11"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -551,12 +760,20 @@
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
     </row>
-    <row r="4" spans="1:30" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="11"/>
+      <c r="B4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="F4" s="11"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -583,12 +800,20 @@
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
     </row>
-    <row r="5" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="11"/>
+      <c r="B5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="F5" s="11"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -647,18 +872,18 @@
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
     </row>
-    <row r="7" spans="1:30" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -711,69 +936,69 @@
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
     </row>
-    <row r="9" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1"/>
-      <c r="AD9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
     </row>
     <row r="10" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-      <c r="AA10" s="2"/>
-      <c r="AB10" s="2"/>
-      <c r="AC10" s="2"/>
-      <c r="AD10" s="2"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
     </row>
     <row r="11" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -809,9 +1034,9 @@
     </row>
     <row r="12" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -875,7 +1100,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -971,7 +1196,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="9"/>
+      <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1035,7 +1260,7 @@
       <c r="A19" s="1"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="10"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1065,9 +1290,9 @@
     </row>
     <row r="20" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1447,69 +1672,69 @@
       <c r="AC31" s="2"/>
       <c r="AD31" s="2"/>
     </row>
-    <row r="32" spans="1:30" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
-      <c r="T32" s="1"/>
-      <c r="U32" s="1"/>
-      <c r="V32" s="1"/>
-      <c r="W32" s="1"/>
-      <c r="X32" s="1"/>
-      <c r="Y32" s="1"/>
-      <c r="Z32" s="1"/>
-      <c r="AA32" s="1"/>
-      <c r="AB32" s="1"/>
-      <c r="AC32" s="1"/>
-      <c r="AD32" s="1"/>
-    </row>
-    <row r="33" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2"/>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="2"/>
+    </row>
+    <row r="33" spans="1:30" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
-      <c r="V33" s="2"/>
-      <c r="W33" s="2"/>
-      <c r="X33" s="2"/>
-      <c r="Y33" s="2"/>
-      <c r="Z33" s="2"/>
-      <c r="AA33" s="2"/>
-      <c r="AB33" s="2"/>
-      <c r="AC33" s="2"/>
-      <c r="AD33" s="2"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="1"/>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="1"/>
+      <c r="AD33" s="1"/>
     </row>
     <row r="34" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
@@ -7369,35 +7594,35 @@
     </row>
     <row r="217" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1"/>
-      <c r="B217" s="1"/>
-      <c r="C217" s="1"/>
-      <c r="D217" s="1"/>
-      <c r="E217" s="1"/>
-      <c r="F217" s="1"/>
-      <c r="G217" s="1"/>
-      <c r="H217" s="1"/>
-      <c r="I217" s="1"/>
-      <c r="J217" s="1"/>
-      <c r="K217" s="1"/>
-      <c r="L217" s="1"/>
-      <c r="M217" s="1"/>
-      <c r="N217" s="1"/>
-      <c r="O217" s="1"/>
-      <c r="P217" s="1"/>
-      <c r="Q217" s="1"/>
-      <c r="R217" s="1"/>
-      <c r="S217" s="1"/>
-      <c r="T217" s="1"/>
-      <c r="U217" s="1"/>
-      <c r="V217" s="1"/>
-      <c r="W217" s="1"/>
-      <c r="X217" s="1"/>
-      <c r="Y217" s="1"/>
-      <c r="Z217" s="1"/>
-      <c r="AA217" s="1"/>
-      <c r="AB217" s="1"/>
-      <c r="AC217" s="1"/>
-      <c r="AD217" s="1"/>
+      <c r="B217" s="2"/>
+      <c r="C217" s="2"/>
+      <c r="D217" s="2"/>
+      <c r="E217" s="2"/>
+      <c r="F217" s="2"/>
+      <c r="G217" s="2"/>
+      <c r="H217" s="2"/>
+      <c r="I217" s="2"/>
+      <c r="J217" s="2"/>
+      <c r="K217" s="2"/>
+      <c r="L217" s="2"/>
+      <c r="M217" s="2"/>
+      <c r="N217" s="2"/>
+      <c r="O217" s="2"/>
+      <c r="P217" s="2"/>
+      <c r="Q217" s="2"/>
+      <c r="R217" s="2"/>
+      <c r="S217" s="2"/>
+      <c r="T217" s="2"/>
+      <c r="U217" s="2"/>
+      <c r="V217" s="2"/>
+      <c r="W217" s="2"/>
+      <c r="X217" s="2"/>
+      <c r="Y217" s="2"/>
+      <c r="Z217" s="2"/>
+      <c r="AA217" s="2"/>
+      <c r="AB217" s="2"/>
+      <c r="AC217" s="2"/>
+      <c r="AD217" s="2"/>
     </row>
     <row r="218" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
@@ -32327,14 +32552,46 @@
       <c r="AC996" s="1"/>
       <c r="AD996" s="1"/>
     </row>
+    <row r="997" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A997" s="1"/>
+      <c r="B997" s="1"/>
+      <c r="C997" s="1"/>
+      <c r="D997" s="1"/>
+      <c r="E997" s="1"/>
+      <c r="F997" s="1"/>
+      <c r="G997" s="1"/>
+      <c r="H997" s="1"/>
+      <c r="I997" s="1"/>
+      <c r="J997" s="1"/>
+      <c r="K997" s="1"/>
+      <c r="L997" s="1"/>
+      <c r="M997" s="1"/>
+      <c r="N997" s="1"/>
+      <c r="O997" s="1"/>
+      <c r="P997" s="1"/>
+      <c r="Q997" s="1"/>
+      <c r="R997" s="1"/>
+      <c r="S997" s="1"/>
+      <c r="T997" s="1"/>
+      <c r="U997" s="1"/>
+      <c r="V997" s="1"/>
+      <c r="W997" s="1"/>
+      <c r="X997" s="1"/>
+      <c r="Y997" s="1"/>
+      <c r="Z997" s="1"/>
+      <c r="AA997" s="1"/>
+      <c r="AB997" s="1"/>
+      <c r="AC997" s="1"/>
+      <c r="AD997" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Feature Type" sqref="C3:C6" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Feature Type" sqref="C6:C7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Technical,Non-Technical"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup fitToHeight="0" orientation="landscape"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C000000Gantt Chart_x000D_</oddHeader>
   </headerFooter>

</xml_diff>

<commit_message>
Updated Project Plan for week 4 Signed-off-by: Ahmed-Zoher <ahmed.o.zoher@gmail.com>
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/Input documents/PO4_DGELV_DIGITAL ELEVATOR_SIQ.xlsx
+++ b/Digital_Elevator_PO4_DGELV/Input documents/PO4_DGELV_DIGITAL ELEVATOR_SIQ.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SWE\clone\Digital_Elevator_PO4_DGELV\Input documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\Input documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC5AC2B-1892-46E5-8478-7870CCF67EA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0324F9-B8EB-4328-A415-51516C9EBF49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2820" yWindow="2820" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PO4_DGELV_Project_Plan" sheetId="1" r:id="rId1"/>
+    <sheet name="PO4_DGELV_SIQ" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -616,7 +616,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -720,7 +720,7 @@
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
     </row>
-    <row r="3" spans="1:30" ht="45.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="30.6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="15" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Update SIQ with answers
</commit_message>
<xml_diff>
--- a/Digital_Elevator_PO4_DGELV/Input documents/PO4_DGELV_DIGITAL ELEVATOR_SIQ.xlsx
+++ b/Digital_Elevator_PO4_DGELV/Input documents/PO4_DGELV_DIGITAL ELEVATOR_SIQ.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\Software Engineering\LOL\Digital_Elevator_PO4_DGELV\Input documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectsWorkSpace\DGELV_Ahmed\Digital_Elevator_PO4_DGELV\Input documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0324F9-B8EB-4328-A415-51516C9EBF49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="2820" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2820" yWindow="2820" windowWidth="17280" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="PO4_DGELV_SIQ" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Initiation Phase</t>
   </si>
@@ -208,11 +207,20 @@
       <t>PO4_DGELV _CYRS_01_V1.2</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">TSH : the idea is to secure the calling of the movement up/down </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSH : the idea is to secure the calling of the movement up/down , it is not about how many floors you have </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSH: the reset is in the input for the user , I think it will be out </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
   </numFmts>
@@ -607,30 +615,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFF2F2F2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AD997"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.36328125" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.7265625" customWidth="1"/>
-    <col min="4" max="4" width="21.90625" customWidth="1"/>
-    <col min="5" max="5" width="34.6328125" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" customWidth="1"/>
-    <col min="8" max="8" width="10.36328125" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" customWidth="1"/>
-    <col min="10" max="11" width="17.6328125" customWidth="1"/>
+    <col min="3" max="3" width="53.77734375" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="10" max="11" width="17.6640625" customWidth="1"/>
     <col min="12" max="30" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -720,7 +728,7 @@
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
     </row>
-    <row r="3" spans="1:30" ht="30.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="54" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="15" t="s">
         <v>21</v>
@@ -735,7 +743,9 @@
         <v>10</v>
       </c>
       <c r="F3" s="11"/>
-      <c r="G3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="H3" s="6"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -775,7 +785,9 @@
         <v>14</v>
       </c>
       <c r="F4" s="11"/>
-      <c r="G4" s="6"/>
+      <c r="G4" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="H4" s="6"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -815,7 +827,9 @@
         <v>12</v>
       </c>
       <c r="F5" s="11"/>
-      <c r="G5" s="6"/>
+      <c r="G5" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="H5" s="6"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -32586,7 +32600,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Feature Type" sqref="C6:C7" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Feature Type" sqref="C6:C7">
       <formula1>"Technical,Non-Technical"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>